<commit_message>
feat: support generate enum types
</commit_message>
<xml_diff>
--- a/example/hero_advance.xlsx
+++ b/example/hero_advance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14780" yWindow="-21140" windowWidth="38400" windowHeight="21140"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,6 +94,30 @@
   </si>
   <si>
     <t>]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ONE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>THREE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TWO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enum&lt;HERO_TYPE|temp&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -420,23 +444,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -479,8 +511,11 @@
       <c r="N2" t="s">
         <v>16</v>
       </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -502,8 +537,11 @@
       <c r="G3" t="s">
         <v>15</v>
       </c>
+      <c r="O3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>104</v>
       </c>
@@ -540,8 +578,11 @@
       <c r="M4">
         <v>4</v>
       </c>
+      <c r="O4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>104</v>
       </c>
@@ -578,8 +619,11 @@
       <c r="M5">
         <v>6</v>
       </c>
+      <c r="O5" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>105</v>
       </c>
@@ -613,8 +657,49 @@
       <c r="L6">
         <v>2</v>
       </c>
+      <c r="O6" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="14" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="O7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>